<commit_message>
added CELH and others
</commit_message>
<xml_diff>
--- a/APLS.xlsx
+++ b/APLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190C01B-2974-41F0-B072-05A1A64BB88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50459951-39FF-4714-B680-077D0DFF7D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50220" yWindow="1860" windowWidth="22875" windowHeight="18315" xr2:uid="{C5D46298-A5E7-4521-8F34-4B6B3EF66A99}"/>
+    <workbookView xWindow="-23220" yWindow="990" windowWidth="22260" windowHeight="19395" activeTab="1" xr2:uid="{C5D46298-A5E7-4521-8F34-4B6B3EF66A99}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Martin Shkreli</author>
+    <author>tc={58C30732-E571-4EAE-B15E-980B4BED0CEB}</author>
   </authors>
   <commentList>
     <comment ref="O3" authorId="0" shapeId="0" xr:uid="{4A806E08-7D69-4C6C-B6F3-F795205259D6}">
@@ -67,12 +68,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="AH3" authorId="1" shapeId="0" xr:uid="{58C30732-E571-4EAE-B15E-980B4BED0CEB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Patent expires 12/2027</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
   <si>
     <t>Price</t>
   </si>
@@ -182,9 +191,6 @@
     <t>Phase III "PEGASUS" n=80 PNH - NCT03050549</t>
   </si>
   <si>
-    <t>Phase III "VALIANT" IC-MPGN/C3G</t>
-  </si>
-  <si>
     <t>Q120</t>
   </si>
   <si>
@@ -417,6 +423,36 @@
   </si>
   <si>
     <t>Q224</t>
+  </si>
+  <si>
+    <t>Q124</t>
+  </si>
+  <si>
+    <t>Q324</t>
+  </si>
+  <si>
+    <t>Q424</t>
+  </si>
+  <si>
+    <t>S/O</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Revenue y/y</t>
+  </si>
+  <si>
+    <t>68% reduction in proteinuria</t>
+  </si>
+  <si>
+    <t>Phase III "VALIANT" n=124 IC-MPGN/C3G</t>
+  </si>
+  <si>
+    <t>APL-3007</t>
+  </si>
+  <si>
+    <t>Phase II HSCT-TMA</t>
   </si>
 </sst>
 </file>
@@ -649,16 +685,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>48986</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>70757</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -673,8 +709,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9492343" y="48986"/>
-          <a:ext cx="0" cy="7532914"/>
+          <a:off x="12578443" y="0"/>
+          <a:ext cx="0" cy="8186057"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -699,15 +735,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>59872</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>59872</xdr:colOff>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>21771</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -723,8 +759,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15027729" y="0"/>
-          <a:ext cx="0" cy="7859485"/>
+          <a:off x="18669001" y="0"/>
+          <a:ext cx="0" cy="8349342"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -748,6 +784,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Martin Shkreli" id="{52505933-672A-481B-9ECE-CD24D7674232}" userId="9ffda80931a57275" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1045,12 +1087,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="AH3" dT="2024-10-10T13:12:29.04" personId="{52505933-672A-481B-9ECE-CD24D7674232}" id="{58C30732-E571-4EAE-B15E-980B4BED0CEB}">
+    <text>Patent expires 12/2027</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6234D1C3-C4BE-43F2-B9DB-E2CAB01F5DB4}">
   <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1095,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>39.75</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2">
@@ -1106,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -1116,7 +1166,7 @@
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I3" s="16"/>
       <c r="K3" t="s">
@@ -1126,12 +1176,12 @@
         <v>121.766328</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1157,7 +1207,7 @@
       </c>
       <c r="L4" s="7">
         <f>L2*L3</f>
-        <v>4840.2115380000005</v>
+        <v>3287.6908560000002</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
@@ -1166,7 +1216,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -1178,15 +1228,15 @@
         <v>360.08699999999999</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
         <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -1200,18 +1250,18 @@
         <v>456.83399999999995</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -1221,30 +1271,32 @@
       </c>
       <c r="L7" s="7">
         <f>+L4-L5+L6</f>
-        <v>4936.9585379999999</v>
+        <v>3384.437856</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="18"/>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L8" s="7">
         <v>2941.5680000000002</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
@@ -1257,10 +1309,10 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L10">
         <v>2009</v>
@@ -1268,20 +1320,20 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G11" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G12" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G13" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
@@ -1289,7 +1341,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G14" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K14" t="s">
         <v>25</v>
@@ -1297,28 +1349,28 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G15" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G16" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="K16" t="s">
         <v>104</v>
-      </c>
-      <c r="K16" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G18" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1332,13 +1384,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E49619-7317-48A8-BEE2-EDC89FDCB0B3}">
-  <dimension ref="A1:AK39"/>
+  <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomRight" activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1348,193 +1400,221 @@
     <col min="3" max="14" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="O2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="W2">
+      <c r="S2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="W2" s="8"/>
+      <c r="AB2">
         <v>2021</v>
       </c>
-      <c r="X2">
-        <f>W2+1</f>
+      <c r="AC2">
+        <f>AB2+1</f>
         <v>2022</v>
       </c>
-      <c r="Y2">
-        <f t="shared" ref="Y2:AK2" si="0">X2+1</f>
+      <c r="AD2">
+        <f t="shared" ref="AD2:AP2" si="0">AC2+1</f>
         <v>2023</v>
       </c>
-      <c r="Z2">
+      <c r="AE2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AA2">
+      <c r="AF2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="AB2">
+      <c r="AG2">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="AC2">
+      <c r="AH2">
         <f t="shared" si="0"/>
         <v>2027</v>
       </c>
-      <c r="AD2">
+      <c r="AI2">
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="AE2">
+      <c r="AJ2">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="AF2">
+      <c r="AK2">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="AG2">
+      <c r="AL2">
         <f t="shared" si="0"/>
         <v>2031</v>
       </c>
-      <c r="AH2">
+      <c r="AM2">
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
-      <c r="AI2">
+      <c r="AN2">
         <f t="shared" si="0"/>
         <v>2033</v>
       </c>
-      <c r="AJ2">
+      <c r="AO2">
         <f t="shared" si="0"/>
         <v>2034</v>
       </c>
-      <c r="AK2">
+      <c r="AP2">
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0</v>
       </c>
       <c r="O3" s="19">
         <v>18.399999999999999</v>
       </c>
       <c r="P3" s="19">
-        <f>O3*4</f>
-        <v>73.599999999999994</v>
+        <v>67.3</v>
       </c>
       <c r="Q3" s="19">
-        <f>P3*1.4</f>
-        <v>103.03999999999999</v>
+        <v>75.3</v>
       </c>
       <c r="R3" s="19">
-        <f>Q3*1.4</f>
-        <v>144.25599999999997</v>
-      </c>
-      <c r="Y3" s="7">
+        <v>114.3</v>
+      </c>
+      <c r="S3" s="19">
+        <v>137.5</v>
+      </c>
+      <c r="T3" s="19">
+        <v>154.6</v>
+      </c>
+      <c r="U3" s="19">
+        <f>+T3+25</f>
+        <v>179.6</v>
+      </c>
+      <c r="V3" s="19">
+        <f>+U3+25</f>
+        <v>204.6</v>
+      </c>
+      <c r="W3" s="19"/>
+      <c r="AD3" s="7">
         <f>SUM(O3:R3)</f>
-        <v>339.29599999999994</v>
-      </c>
-      <c r="Z3" s="7">
-        <f>Y3*2.1</f>
-        <v>712.52159999999992</v>
-      </c>
-      <c r="AA3" s="7">
-        <f>Z3*1.5</f>
-        <v>1068.7823999999998</v>
-      </c>
-      <c r="AB3" s="7">
-        <f>AA3*1.1</f>
-        <v>1175.6606399999998</v>
-      </c>
-      <c r="AC3" s="7">
-        <f>AB3*1.1</f>
-        <v>1293.2267039999999</v>
-      </c>
-      <c r="AD3" s="7">
-        <f>AC3*1.1</f>
-        <v>1422.5493744</v>
+        <v>275.3</v>
       </c>
       <c r="AE3" s="7">
-        <f>AD3*1.05</f>
-        <v>1493.6768431200001</v>
+        <f>SUM(S3:V3)</f>
+        <v>676.30000000000007</v>
       </c>
       <c r="AF3" s="7">
-        <f t="shared" ref="AF3:AH3" si="1">AE3*1.05</f>
-        <v>1568.3606852760001</v>
+        <f>AE3*1.5</f>
+        <v>1014.45</v>
       </c>
       <c r="AG3" s="7">
+        <f>AF3*1.1</f>
+        <v>1115.8950000000002</v>
+      </c>
+      <c r="AH3" s="7">
+        <f>AG3*1.1</f>
+        <v>1227.4845000000003</v>
+      </c>
+      <c r="AI3" s="7">
+        <f>+AH3*0.5</f>
+        <v>613.74225000000013</v>
+      </c>
+      <c r="AJ3" s="7">
+        <f t="shared" ref="AJ3:AP3" si="1">+AI3*0.1</f>
+        <v>61.374225000000017</v>
+      </c>
+      <c r="AK3" s="7">
         <f t="shared" si="1"/>
-        <v>1646.7787195398002</v>
-      </c>
-      <c r="AH3" s="7">
+        <v>6.1374225000000022</v>
+      </c>
+      <c r="AL3" s="7">
         <f t="shared" si="1"/>
-        <v>1729.1176555167904</v>
-      </c>
-      <c r="AI3" s="7">
-        <f>AH3*0.99</f>
-        <v>1711.8264789616223</v>
-      </c>
-      <c r="AJ3" s="7">
-        <f t="shared" ref="AJ3:AK3" si="2">AI3*0.99</f>
-        <v>1694.7082141720061</v>
-      </c>
-      <c r="AK3" s="7">
-        <f t="shared" si="2"/>
-        <v>1677.761132030286</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.61374225000000027</v>
+      </c>
+      <c r="AM3" s="7">
+        <f t="shared" si="1"/>
+        <v>6.1374225000000032E-2</v>
+      </c>
+      <c r="AN3" s="7">
+        <f t="shared" si="1"/>
+        <v>6.1374225000000032E-3</v>
+      </c>
+      <c r="AO3" s="7">
+        <f t="shared" si="1"/>
+        <v>6.1374225000000032E-4</v>
+      </c>
+      <c r="AP3" s="7">
+        <f t="shared" si="1"/>
+        <v>6.1374225000000035E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
@@ -1553,7 +1633,9 @@
       </c>
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+      <c r="N4" s="19">
+        <v>19.7</v>
+      </c>
       <c r="O4" s="7">
         <v>20.399999999999999</v>
       </c>
@@ -1562,69 +1644,81 @@
         <v>22.4</v>
       </c>
       <c r="Q4" s="7">
-        <f>P4+2</f>
+        <v>23.9</v>
+      </c>
+      <c r="R4" s="7">
         <v>24.4</v>
       </c>
-      <c r="R4" s="7">
-        <f>Q4+2</f>
-        <v>26.4</v>
-      </c>
-      <c r="Y4" s="7">
+      <c r="S4" s="7">
+        <v>25.6</v>
+      </c>
+      <c r="T4" s="7">
+        <v>24.5</v>
+      </c>
+      <c r="U4" s="7">
+        <f>+T4+1</f>
+        <v>25.5</v>
+      </c>
+      <c r="V4" s="7">
+        <f>+U4+1</f>
+        <v>26.5</v>
+      </c>
+      <c r="AD4" s="7">
         <f>SUM(O4:R4)</f>
-        <v>93.6</v>
-      </c>
-      <c r="Z4" s="7">
-        <f>Y4*1.01</f>
-        <v>94.536000000000001</v>
-      </c>
-      <c r="AA4" s="7">
-        <f t="shared" ref="AA4:AK4" si="3">Z4*1.01</f>
-        <v>95.481359999999995</v>
-      </c>
-      <c r="AB4" s="7">
-        <f t="shared" si="3"/>
-        <v>96.436173599999989</v>
-      </c>
-      <c r="AC4" s="7">
-        <f t="shared" si="3"/>
-        <v>97.40053533599999</v>
-      </c>
-      <c r="AD4" s="7">
-        <f t="shared" si="3"/>
-        <v>98.374540689359989</v>
+        <v>91.1</v>
       </c>
       <c r="AE4" s="7">
-        <f t="shared" si="3"/>
-        <v>99.358286096253593</v>
+        <f>SUM(S4:V4)</f>
+        <v>102.1</v>
       </c>
       <c r="AF4" s="7">
-        <f t="shared" si="3"/>
-        <v>100.35186895721613</v>
+        <f t="shared" ref="AF4:AP4" si="2">AE4*1.01</f>
+        <v>103.121</v>
       </c>
       <c r="AG4" s="7">
-        <f t="shared" si="3"/>
-        <v>101.35538764678829</v>
+        <f t="shared" si="2"/>
+        <v>104.15221</v>
       </c>
       <c r="AH4" s="7">
-        <f t="shared" si="3"/>
-        <v>102.36894152325617</v>
+        <f t="shared" si="2"/>
+        <v>105.19373209999999</v>
       </c>
       <c r="AI4" s="7">
-        <f t="shared" si="3"/>
-        <v>103.39263093848874</v>
+        <f t="shared" si="2"/>
+        <v>106.24566942099999</v>
       </c>
       <c r="AJ4" s="7">
-        <f t="shared" si="3"/>
-        <v>104.42655724787362</v>
+        <f t="shared" si="2"/>
+        <v>107.30812611520999</v>
       </c>
       <c r="AK4" s="7">
-        <f t="shared" si="3"/>
-        <v>105.47082282035235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>108.38120737636208</v>
+      </c>
+      <c r="AL4" s="7">
+        <f t="shared" si="2"/>
+        <v>109.46501945012571</v>
+      </c>
+      <c r="AM4" s="7">
+        <f t="shared" si="2"/>
+        <v>110.55966964462696</v>
+      </c>
+      <c r="AN4" s="7">
+        <f t="shared" si="2"/>
+        <v>111.66526634107323</v>
+      </c>
+      <c r="AO4" s="7">
+        <f t="shared" si="2"/>
+        <v>112.78191900448397</v>
+      </c>
+      <c r="AP4" s="7">
+        <f t="shared" si="2"/>
+        <v>113.90973819452881</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -1637,18 +1731,39 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="N5" s="19">
+        <v>3.01</v>
+      </c>
       <c r="O5" s="7">
         <v>6.0460000000000003</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="P5" s="7">
+        <v>5.3239999999999998</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>11.217000000000001</v>
+      </c>
+      <c r="R5" s="7">
+        <v>7.7220000000000004</v>
+      </c>
+      <c r="S5" s="7">
+        <v>9.25</v>
+      </c>
+      <c r="T5" s="7">
+        <v>20.548999999999999</v>
+      </c>
+      <c r="AD5" s="7">
         <f>SUM(O5:R5)</f>
-        <v>6.0460000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>30.309000000000005</v>
+      </c>
+      <c r="AE5" s="7">
+        <f>SUM(S5:V5)</f>
+        <v>29.798999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -1661,79 +1776,98 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+      <c r="N6" s="20">
+        <f>N4+N5+N3</f>
+        <v>22.71</v>
+      </c>
       <c r="O6" s="20">
         <f>O4+O5+O3</f>
         <v>44.845999999999997</v>
       </c>
       <c r="P6" s="20">
         <f>P4+P5+P3</f>
-        <v>96</v>
+        <v>95.024000000000001</v>
       </c>
       <c r="Q6" s="20">
-        <f t="shared" ref="Q6:R6" si="4">Q4+Q5+Q3</f>
-        <v>127.44</v>
+        <f t="shared" ref="Q6:V6" si="3">Q4+Q5+Q3</f>
+        <v>110.417</v>
       </c>
       <c r="R6" s="20">
+        <f t="shared" si="3"/>
+        <v>146.422</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="3"/>
+        <v>172.35</v>
+      </c>
+      <c r="T6" s="20">
+        <f t="shared" si="3"/>
+        <v>199.649</v>
+      </c>
+      <c r="U6" s="20">
+        <f t="shared" si="3"/>
+        <v>205.1</v>
+      </c>
+      <c r="V6" s="20">
+        <f t="shared" si="3"/>
+        <v>231.1</v>
+      </c>
+      <c r="AD6" s="20">
+        <f>SUM(AD3:AD5)</f>
+        <v>396.709</v>
+      </c>
+      <c r="AE6" s="20">
+        <f t="shared" ref="AE6:AP6" si="4">SUM(AE3:AE5)</f>
+        <v>808.19900000000007</v>
+      </c>
+      <c r="AF6" s="20">
         <f t="shared" si="4"/>
-        <v>170.65599999999998</v>
-      </c>
-      <c r="Y6" s="20">
-        <f>SUM(Y3:Y5)</f>
-        <v>438.94199999999995</v>
-      </c>
-      <c r="Z6" s="20">
-        <f t="shared" ref="Z6:AK6" si="5">SUM(Z3:Z5)</f>
-        <v>807.05759999999987</v>
-      </c>
-      <c r="AA6" s="20">
-        <f t="shared" si="5"/>
-        <v>1164.2637599999998</v>
-      </c>
-      <c r="AB6" s="20">
-        <f t="shared" si="5"/>
-        <v>1272.0968135999999</v>
-      </c>
-      <c r="AC6" s="20">
-        <f t="shared" si="5"/>
-        <v>1390.627239336</v>
-      </c>
-      <c r="AD6" s="20">
-        <f t="shared" si="5"/>
-        <v>1520.92391508936</v>
-      </c>
-      <c r="AE6" s="20">
-        <f t="shared" si="5"/>
-        <v>1593.0351292162536</v>
-      </c>
-      <c r="AF6" s="20">
-        <f t="shared" si="5"/>
-        <v>1668.7125542332162</v>
+        <v>1117.5710000000001</v>
       </c>
       <c r="AG6" s="20">
-        <f t="shared" si="5"/>
-        <v>1748.1341071865886</v>
+        <f t="shared" si="4"/>
+        <v>1220.0472100000002</v>
       </c>
       <c r="AH6" s="20">
-        <f t="shared" si="5"/>
-        <v>1831.4865970400465</v>
+        <f t="shared" si="4"/>
+        <v>1332.6782321000003</v>
       </c>
       <c r="AI6" s="20">
-        <f t="shared" si="5"/>
-        <v>1815.2191099001111</v>
+        <f t="shared" si="4"/>
+        <v>719.98791942100013</v>
       </c>
       <c r="AJ6" s="20">
-        <f t="shared" si="5"/>
-        <v>1799.1347714198798</v>
+        <f t="shared" si="4"/>
+        <v>168.68235111521</v>
       </c>
       <c r="AK6" s="20">
-        <f t="shared" si="5"/>
-        <v>1783.2319548506384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>114.51862987636208</v>
+      </c>
+      <c r="AL6" s="20">
+        <f t="shared" si="4"/>
+        <v>110.07876170012571</v>
+      </c>
+      <c r="AM6" s="20">
+        <f t="shared" si="4"/>
+        <v>110.62104386962696</v>
+      </c>
+      <c r="AN6" s="20">
+        <f t="shared" si="4"/>
+        <v>111.67140376357324</v>
+      </c>
+      <c r="AO6" s="20">
+        <f t="shared" si="4"/>
+        <v>112.78253274673396</v>
+      </c>
+      <c r="AP6" s="20">
+        <f t="shared" si="4"/>
+        <v>113.90979956875381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1746,30 +1880,47 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="N7" s="19">
+        <v>2.9249999999999998</v>
+      </c>
       <c r="O7" s="7">
         <v>7.8090000000000002</v>
       </c>
       <c r="P7" s="7">
-        <f>P6-P8</f>
-        <v>14.400000000000006</v>
+        <v>8.3789999999999996</v>
       </c>
       <c r="Q7" s="7">
-        <f t="shared" ref="Q7:R7" si="6">Q6-Q8</f>
-        <v>19.116</v>
+        <v>22.41</v>
       </c>
       <c r="R7" s="7">
-        <f t="shared" si="6"/>
-        <v>25.598399999999998</v>
-      </c>
-      <c r="Y7" s="7">
+        <v>19.911999999999999</v>
+      </c>
+      <c r="S7" s="7">
+        <v>20.209</v>
+      </c>
+      <c r="T7" s="7">
+        <v>23.1</v>
+      </c>
+      <c r="U7" s="7">
+        <f>+U6-U8</f>
+        <v>20.509999999999991</v>
+      </c>
+      <c r="V7" s="7">
+        <f>+V6-V8</f>
+        <v>23.109999999999985</v>
+      </c>
+      <c r="AD7" s="7">
         <f>SUM(O7:R7)</f>
-        <v>66.923400000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>58.51</v>
+      </c>
+      <c r="AE7" s="7">
+        <f>SUM(S7:V7)</f>
+        <v>86.928999999999974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1782,31 +1933,66 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="N8" s="19">
+        <f>+N6-N7</f>
+        <v>19.785</v>
+      </c>
       <c r="O8" s="7">
         <f>O6-O7</f>
         <v>37.036999999999999</v>
       </c>
       <c r="P8" s="7">
         <f>P6*0.85</f>
-        <v>81.599999999999994</v>
+        <v>80.770399999999995</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" ref="Q8:R8" si="7">Q6*0.85</f>
-        <v>108.324</v>
+        <f>+Q6-Q7</f>
+        <v>88.007000000000005</v>
       </c>
       <c r="R8" s="7">
-        <f t="shared" si="7"/>
-        <v>145.05759999999998</v>
-      </c>
-      <c r="Y8" s="7">
-        <f>Y6-Y7</f>
-        <v>372.01859999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <f>+R6-R7</f>
+        <v>126.50999999999999</v>
+      </c>
+      <c r="S8" s="7">
+        <f>+S6-S7</f>
+        <v>152.14099999999999</v>
+      </c>
+      <c r="T8" s="7">
+        <f>+T6-T7</f>
+        <v>176.54900000000001</v>
+      </c>
+      <c r="U8" s="7">
+        <f>+U6*0.9</f>
+        <v>184.59</v>
+      </c>
+      <c r="V8" s="7">
+        <f>+V6*0.9</f>
+        <v>207.99</v>
+      </c>
+      <c r="AD8" s="7">
+        <f>+AD6-AD7</f>
+        <v>338.19900000000001</v>
+      </c>
+      <c r="AE8" s="7">
+        <f>+AE6-AE7</f>
+        <v>721.2700000000001</v>
+      </c>
+      <c r="AF8" s="7">
+        <f>+AF6*0.9</f>
+        <v>1005.8139000000001</v>
+      </c>
+      <c r="AG8" s="7">
+        <f>+AG6*0.9</f>
+        <v>1098.0424890000002</v>
+      </c>
+      <c r="AH8" s="7">
+        <f>+AH6*0.9</f>
+        <v>1199.4104088900003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1819,14 +2005,39 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="N9" s="19">
+        <v>99.423000000000002</v>
+      </c>
       <c r="O9" s="7">
         <v>110.027</v>
       </c>
-    </row>
-    <row r="10" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P9" s="7">
+        <v>95.658000000000001</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>79.421000000000006</v>
+      </c>
+      <c r="R9" s="7">
+        <v>69.281999999999996</v>
+      </c>
+      <c r="S9" s="7">
+        <v>84.700999999999993</v>
+      </c>
+      <c r="T9" s="7">
+        <v>77.947000000000003</v>
+      </c>
+      <c r="AD9" s="7">
+        <f>SUM(O9:R9)</f>
+        <v>354.38799999999998</v>
+      </c>
+      <c r="AE9" s="7">
+        <f>SUM(S9:V9)</f>
+        <v>162.648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1839,26 +2050,59 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="N10" s="19">
+        <v>84.367999999999995</v>
+      </c>
       <c r="O10" s="7">
         <v>102.093</v>
       </c>
       <c r="P10" s="7">
-        <f>O10</f>
-        <v>102.093</v>
+        <v>111.373</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" ref="Q10:R10" si="8">P10</f>
-        <v>102.093</v>
+        <v>145.648</v>
       </c>
       <c r="R10" s="7">
-        <f t="shared" si="8"/>
-        <v>102.093</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>141.70099999999999</v>
+      </c>
+      <c r="S10" s="7">
+        <v>129.505</v>
+      </c>
+      <c r="T10" s="7">
+        <v>128.08099999999999</v>
+      </c>
+      <c r="U10" s="7">
+        <f>+Q10</f>
+        <v>145.648</v>
+      </c>
+      <c r="V10" s="7">
+        <f>+R10</f>
+        <v>141.70099999999999</v>
+      </c>
+      <c r="AD10" s="7">
+        <f>SUM(O10:R10)</f>
+        <v>500.81500000000005</v>
+      </c>
+      <c r="AE10" s="7">
+        <f>SUM(S10:V10)</f>
+        <v>544.93500000000006</v>
+      </c>
+      <c r="AF10" s="7">
+        <f>+AE10*0.5</f>
+        <v>272.46750000000003</v>
+      </c>
+      <c r="AG10" s="7">
+        <f>+AF10*0.5</f>
+        <v>136.23375000000001</v>
+      </c>
+      <c r="AH10" s="7">
+        <f>+AG10*0.5</f>
+        <v>68.116875000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1871,27 +2115,66 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="N11" s="7">
+        <f>N9+N10</f>
+        <v>183.791</v>
+      </c>
       <c r="O11" s="7">
         <f>O9+O10</f>
         <v>212.12</v>
       </c>
       <c r="P11" s="7">
-        <f t="shared" ref="P11:R11" si="9">P9+P10</f>
-        <v>102.093</v>
+        <f t="shared" ref="P11:R11" si="5">P9+P10</f>
+        <v>207.03100000000001</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="9"/>
-        <v>102.093</v>
+        <f t="shared" si="5"/>
+        <v>225.06900000000002</v>
       </c>
       <c r="R11" s="7">
-        <f t="shared" si="9"/>
-        <v>102.093</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>210.983</v>
+      </c>
+      <c r="S11" s="7">
+        <f>+S9+S10</f>
+        <v>214.20599999999999</v>
+      </c>
+      <c r="T11" s="7">
+        <f>+T9+T10</f>
+        <v>206.02799999999999</v>
+      </c>
+      <c r="U11" s="7">
+        <f t="shared" ref="U11:V11" si="6">+U9+U10</f>
+        <v>145.648</v>
+      </c>
+      <c r="V11" s="7">
+        <f t="shared" si="6"/>
+        <v>141.70099999999999</v>
+      </c>
+      <c r="AD11" s="7">
+        <f>+AD10+AD9</f>
+        <v>855.20299999999997</v>
+      </c>
+      <c r="AE11" s="7">
+        <f>+AE10+AE9</f>
+        <v>707.58300000000008</v>
+      </c>
+      <c r="AF11" s="7">
+        <f t="shared" ref="AF11:AG11" si="7">+AF10+AF9</f>
+        <v>272.46750000000003</v>
+      </c>
+      <c r="AG11" s="7">
+        <f t="shared" si="7"/>
+        <v>136.23375000000001</v>
+      </c>
+      <c r="AH11" s="7">
+        <f t="shared" ref="AH11" si="8">+AH10+AH9</f>
+        <v>68.116875000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -1904,27 +2187,66 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+      <c r="N12" s="7">
+        <f>N8-N11</f>
+        <v>-164.006</v>
+      </c>
       <c r="O12" s="7">
         <f>O8-O11</f>
         <v>-175.083</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" ref="P12:R12" si="10">P8-P11</f>
-        <v>-20.493000000000009</v>
+        <f t="shared" ref="P12:R12" si="9">P8-P11</f>
+        <v>-126.26060000000001</v>
       </c>
       <c r="Q12" s="7">
+        <f t="shared" si="9"/>
+        <v>-137.06200000000001</v>
+      </c>
+      <c r="R12" s="7">
+        <f t="shared" si="9"/>
+        <v>-84.473000000000013</v>
+      </c>
+      <c r="S12" s="7">
+        <f>+S8-S11</f>
+        <v>-62.064999999999998</v>
+      </c>
+      <c r="T12" s="7">
+        <f>+T8-T11</f>
+        <v>-29.478999999999985</v>
+      </c>
+      <c r="U12" s="7">
+        <f t="shared" ref="U12:V12" si="10">+U8-U11</f>
+        <v>38.942000000000007</v>
+      </c>
+      <c r="V12" s="7">
         <f t="shared" si="10"/>
-        <v>6.2309999999999945</v>
-      </c>
-      <c r="R12" s="7">
-        <f t="shared" si="10"/>
-        <v>42.964599999999976</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>66.289000000000016</v>
+      </c>
+      <c r="AD12" s="7">
+        <f>+AD8-AD11</f>
+        <v>-517.00399999999991</v>
+      </c>
+      <c r="AE12" s="7">
+        <f>+AE8-AE11</f>
+        <v>13.687000000000012</v>
+      </c>
+      <c r="AF12" s="7">
+        <f t="shared" ref="AF12:AG12" si="11">+AF8-AF11</f>
+        <v>733.34640000000013</v>
+      </c>
+      <c r="AG12" s="7">
+        <f t="shared" si="11"/>
+        <v>961.80873900000017</v>
+      </c>
+      <c r="AH12" s="7">
+        <f t="shared" ref="AH12" si="12">+AH8-AH11</f>
+        <v>1131.2935338900004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -1937,15 +2259,46 @@
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="N13" s="19">
+        <f>4.575-7.738</f>
+        <v>-3.1630000000000003</v>
+      </c>
       <c r="O13" s="7">
         <f>5.393-7.529-0.277</f>
         <v>-2.4130000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P13" s="7">
+        <f>6.002-7.341</f>
+        <v>-1.3390000000000004</v>
+      </c>
+      <c r="Q13" s="7">
+        <f>4.989-7.31</f>
+        <v>-2.3209999999999997</v>
+      </c>
+      <c r="R13" s="7">
+        <f>-7.402+4.548</f>
+        <v>-2.8540000000000001</v>
+      </c>
+      <c r="S13" s="7">
+        <f>3.303-6.967</f>
+        <v>-3.6639999999999997</v>
+      </c>
+      <c r="T13" s="7">
+        <f>3.184-9.359</f>
+        <v>-6.1749999999999998</v>
+      </c>
+      <c r="AD13" s="7">
+        <f>SUM(O13:R13)</f>
+        <v>-8.9269999999999996</v>
+      </c>
+      <c r="AE13" s="7">
+        <f>SUM(S13:V13)</f>
+        <v>-9.8389999999999986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1958,27 +2311,66 @@
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="N14" s="7">
+        <f>N12+N13</f>
+        <v>-167.16900000000001</v>
+      </c>
       <c r="O14" s="7">
         <f>O12+O13</f>
         <v>-177.49600000000001</v>
       </c>
       <c r="P14" s="7">
-        <f t="shared" ref="P14:R14" si="11">P12+P13</f>
-        <v>-20.493000000000009</v>
+        <f t="shared" ref="P14:R14" si="13">P12+P13</f>
+        <v>-127.59960000000001</v>
       </c>
       <c r="Q14" s="7">
-        <f t="shared" si="11"/>
-        <v>6.2309999999999945</v>
+        <f t="shared" si="13"/>
+        <v>-139.38300000000001</v>
       </c>
       <c r="R14" s="7">
-        <f t="shared" si="11"/>
-        <v>42.964599999999976</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="13"/>
+        <v>-87.327000000000012</v>
+      </c>
+      <c r="S14" s="7">
+        <f>+S12+S13</f>
+        <v>-65.728999999999999</v>
+      </c>
+      <c r="T14" s="7">
+        <f>+T12+T13</f>
+        <v>-35.653999999999982</v>
+      </c>
+      <c r="U14" s="7">
+        <f>+U12+U13</f>
+        <v>38.942000000000007</v>
+      </c>
+      <c r="V14" s="7">
+        <f>+V12+V13</f>
+        <v>66.289000000000016</v>
+      </c>
+      <c r="AD14" s="7">
+        <f>+AD12+AD13</f>
+        <v>-525.93099999999993</v>
+      </c>
+      <c r="AE14" s="7">
+        <f>+AE12+AE13</f>
+        <v>3.8480000000000132</v>
+      </c>
+      <c r="AF14" s="7">
+        <f t="shared" ref="AF14:AG14" si="14">+AF12+AF13</f>
+        <v>733.34640000000013</v>
+      </c>
+      <c r="AG14" s="7">
+        <f t="shared" si="14"/>
+        <v>961.80873900000017</v>
+      </c>
+      <c r="AH14" s="7">
+        <f t="shared" ref="AH14" si="15">+AH12+AH13</f>
+        <v>1131.2935338900004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -1991,14 +2383,51 @@
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="N15" s="7">
+        <v>0.28199999999999997</v>
+      </c>
       <c r="O15" s="7">
         <v>0.28199999999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P15" s="7">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="R15" s="7">
+        <v>1.423</v>
+      </c>
+      <c r="S15" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="T15" s="7">
+        <v>0.114</v>
+      </c>
+      <c r="AD15" s="7">
+        <f>SUM(O15:R15)</f>
+        <v>2.1320000000000001</v>
+      </c>
+      <c r="AE15" s="7">
+        <f>SUM(S15:V15)</f>
+        <v>0.28400000000000003</v>
+      </c>
+      <c r="AF15" s="7">
+        <f>+AF14*0.1</f>
+        <v>73.334640000000022</v>
+      </c>
+      <c r="AG15" s="7">
+        <f>+AG14*0.2</f>
+        <v>192.36174780000005</v>
+      </c>
+      <c r="AH15" s="7">
+        <f>+AH14*0.2</f>
+        <v>226.25870677800009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -2011,200 +2440,404 @@
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="N16" s="7">
+        <v>-1.4710000000000001</v>
+      </c>
       <c r="O16" s="7">
         <f>O14-O15</f>
         <v>-177.77800000000002</v>
       </c>
       <c r="P16" s="7">
-        <f t="shared" ref="P16:R16" si="12">P14-P15</f>
-        <v>-20.493000000000009</v>
+        <f t="shared" ref="P16:R16" si="16">P14-P15</f>
+        <v>-127.79360000000001</v>
       </c>
       <c r="Q16" s="7">
-        <f t="shared" si="12"/>
-        <v>6.2309999999999945</v>
+        <f t="shared" si="16"/>
+        <v>-139.61600000000001</v>
       </c>
       <c r="R16" s="7">
-        <f t="shared" si="12"/>
-        <v>42.964599999999976</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="16"/>
+        <v>-88.750000000000014</v>
+      </c>
+      <c r="S16" s="7">
+        <f>+S14-S15</f>
+        <v>-65.899000000000001</v>
+      </c>
+      <c r="T16" s="7">
+        <f>+T14-T15</f>
+        <v>-35.767999999999979</v>
+      </c>
+      <c r="U16" s="7">
+        <f>+U14-U15</f>
+        <v>38.942000000000007</v>
+      </c>
+      <c r="V16" s="7">
+        <f>+V14-V15</f>
+        <v>66.289000000000016</v>
+      </c>
+      <c r="AD16" s="7">
+        <f>+AD14-AD15</f>
+        <v>-528.06299999999987</v>
+      </c>
+      <c r="AE16" s="7">
+        <f>+AE14-AE15</f>
+        <v>3.5640000000000134</v>
+      </c>
+      <c r="AF16" s="7">
+        <f t="shared" ref="AF16:AG16" si="17">+AF14-AF15</f>
+        <v>660.01176000000009</v>
+      </c>
+      <c r="AG16" s="7">
+        <f t="shared" si="17"/>
+        <v>769.44699120000018</v>
+      </c>
+      <c r="AH16" s="7">
+        <f t="shared" ref="AH16" si="18">+AH14-AH15</f>
+        <v>905.03482711200036</v>
+      </c>
+    </row>
+    <row r="17" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N17" s="1">
+        <f>+N16/N18</f>
+        <v>-1.3296694356814217E-2</v>
+      </c>
+      <c r="O17" s="1">
+        <f>+O16/O18</f>
+        <v>-1.561209076858227</v>
+      </c>
+      <c r="P17" s="1">
+        <f>+P16/P18</f>
+        <v>-1.0710516611351371</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>+Q16/Q18</f>
+        <v>-1.1606424367372727</v>
+      </c>
+      <c r="R17" s="1">
+        <f>+R16/R18</f>
+        <v>-0.73206744093968601</v>
+      </c>
+      <c r="S17" s="1">
+        <f>+S16/S18</f>
+        <v>-0.53595159283326699</v>
+      </c>
+      <c r="T17" s="1">
+        <f>+T16/T18</f>
+        <v>-0.28867510330578494</v>
+      </c>
+      <c r="U17" s="1">
+        <f>+U16/U18</f>
+        <v>0.31429170971074388</v>
+      </c>
+      <c r="V17" s="1">
+        <f>+V16/V18</f>
+        <v>0.53500290547520679</v>
+      </c>
+      <c r="AD17" s="1">
+        <f t="shared" ref="AD17:AH17" si="19">+AD16/AD18</f>
+        <v>-4.4495441446603401</v>
+      </c>
+      <c r="AE17" s="1">
+        <f t="shared" si="19"/>
+        <v>2.8819271068128493E-2</v>
+      </c>
+      <c r="AF17" s="1">
+        <f t="shared" si="19"/>
+        <v>5.3369971435444725</v>
+      </c>
+      <c r="AG17" s="1">
+        <f t="shared" si="19"/>
+        <v>6.2219139764165554</v>
+      </c>
+      <c r="AH17" s="1">
+        <f t="shared" si="19"/>
+        <v>7.3183063997299236</v>
+      </c>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O18" s="23">
+        <v>117</v>
+      </c>
+      <c r="N18" s="7">
+        <v>110.629</v>
+      </c>
+      <c r="O18" s="7">
+        <v>113.872</v>
+      </c>
+      <c r="P18" s="7">
+        <v>119.316</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>120.292</v>
+      </c>
+      <c r="R18" s="7">
+        <v>121.232</v>
+      </c>
+      <c r="S18" s="7">
+        <v>122.95699999999999</v>
+      </c>
+      <c r="T18" s="7">
+        <v>123.904</v>
+      </c>
+      <c r="U18" s="7">
+        <f>+T18</f>
+        <v>123.904</v>
+      </c>
+      <c r="V18" s="7">
+        <f>+U18</f>
+        <v>123.904</v>
+      </c>
+      <c r="AD18" s="7">
+        <f>AVERAGE(O18:R18)</f>
+        <v>118.678</v>
+      </c>
+      <c r="AE18" s="7">
+        <f>AVERAGE(S18:V18)</f>
+        <v>123.66725</v>
+      </c>
+      <c r="AF18" s="7">
+        <f>+AE18</f>
+        <v>123.66725</v>
+      </c>
+      <c r="AG18" s="7">
+        <f>+AF18</f>
+        <v>123.66725</v>
+      </c>
+      <c r="AH18" s="7">
+        <f t="shared" ref="AH18" si="20">+AG18</f>
+        <v>123.66725</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B19" s="7"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23">
+        <f>+R6/N6-1</f>
+        <v>5.44746807573756</v>
+      </c>
+      <c r="S20" s="23">
+        <f>+S6/O6-1</f>
+        <v>2.8431521205904655</v>
+      </c>
+      <c r="T20" s="23">
+        <f>+T6/P6-1</f>
+        <v>1.1010376325980804</v>
+      </c>
+      <c r="U20" s="23">
+        <f>+U6/Q6-1</f>
+        <v>0.85750382640354283</v>
+      </c>
+      <c r="V20" s="23">
+        <f>+V6/R6-1</f>
+        <v>0.57831473412465328</v>
+      </c>
+    </row>
+    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N21" s="23">
+        <f>N8/N6</f>
+        <v>0.87120211360634081</v>
+      </c>
+      <c r="O21" s="23">
         <f>O8/O6</f>
         <v>0.82587075770414309</v>
       </c>
-      <c r="P18" s="23">
-        <f t="shared" ref="P18:R18" si="13">P8/P6</f>
+      <c r="P21" s="23">
+        <f t="shared" ref="P21:V21" si="21">P8/P6</f>
         <v>0.85</v>
       </c>
-      <c r="Q18" s="23">
-        <f t="shared" si="13"/>
-        <v>0.85</v>
-      </c>
-      <c r="R18" s="23">
-        <f t="shared" si="13"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="O20" s="7">
-        <f>O21-O35</f>
+      <c r="Q21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.79704212213698977</v>
+      </c>
+      <c r="R21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.86400950676810861</v>
+      </c>
+      <c r="S21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.88274441543371041</v>
+      </c>
+      <c r="T21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.88429694113168611</v>
+      </c>
+      <c r="U21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.9</v>
+      </c>
+      <c r="V21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.9</v>
+      </c>
+      <c r="W21" s="23"/>
+    </row>
+    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O23" s="7">
+        <f>O24-O38</f>
         <v>673.54899999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>10</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O24" s="7">
         <f>765.083+1.275</f>
         <v>766.35799999999995</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="O25" s="7">
+        <v>31.504999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="O22" s="7">
-        <v>31.504999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="O26" s="7">
+        <v>85.483999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="O23" s="7">
-        <v>85.483999999999995</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="O27" s="7">
+        <v>36.558999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>75</v>
       </c>
-      <c r="O24" s="7">
-        <v>36.558999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="O28" s="7">
+        <v>34.348999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="7">
-        <v>34.348999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="O29" s="7">
+        <v>17.853999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>77</v>
       </c>
-      <c r="O26" s="7">
-        <v>17.853999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="O30" s="7">
+        <v>5.9669999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="7">
-        <v>5.9669999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="O31" s="7">
+        <v>0.79300000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>79</v>
       </c>
-      <c r="O28" s="7">
-        <v>0.79300000000000004</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>80</v>
-      </c>
-      <c r="O29" s="7">
-        <f>SUM(O21:O28)</f>
+      <c r="O32" s="7">
+        <f>SUM(O24:O31)</f>
         <v>978.86900000000003</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="O30" s="7"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="O34" s="7">
+        <v>31.494</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>83</v>
       </c>
-      <c r="O31" s="7">
-        <v>31.494</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="O35" s="7">
+        <v>71.251000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>84</v>
       </c>
-      <c r="O32" s="7">
-        <v>71.251000000000005</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>85</v>
-      </c>
-      <c r="O33" s="7">
+      <c r="O36" s="7">
         <f>30.071+321.713</f>
         <v>351.78400000000005</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>77</v>
-      </c>
-      <c r="O34" s="7">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="O37" s="7">
         <f>5.828+13.233</f>
         <v>19.061</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="O35" s="7">
-        <v>92.808999999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="O36" s="7">
-        <v>0.34699999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>82</v>
-      </c>
-      <c r="O37" s="7">
-        <v>412.12299999999999</v>
-      </c>
-    </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="O38" s="7">
+        <v>92.808999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="O39" s="7">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>81</v>
       </c>
-      <c r="O38" s="7">
-        <f>SUM(O31:O37)</f>
+      <c r="O40" s="7">
+        <v>412.12299999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="O41" s="7">
+        <f>SUM(O34:O40)</f>
         <v>978.86899999999991</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="O39" s="7"/>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O42" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2218,9 +2851,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDEC44E-3A9A-47B3-8A31-8E621049E97B}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2278,7 +2913,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2296,19 +2931,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C16" s="10" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" s="10" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2341,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2349,23 +2994,23 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
         <v>98</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2375,12 +3020,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2390,7 +3035,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
AMC, APLS, NVS updates, some new models
</commit_message>
<xml_diff>
--- a/APLS.xlsx
+++ b/APLS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50459951-39FF-4714-B680-077D0DFF7D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F72DD0-AFB7-412D-A43C-EFC03D42F8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23220" yWindow="990" windowWidth="22260" windowHeight="19395" activeTab="1" xr2:uid="{C5D46298-A5E7-4521-8F34-4B6B3EF66A99}"/>
+    <workbookView xWindow="-49470" yWindow="2400" windowWidth="32550" windowHeight="17250" activeTab="2" xr2:uid="{C5D46298-A5E7-4521-8F34-4B6B3EF66A99}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="127">
   <si>
     <t>Price</t>
   </si>
@@ -453,6 +453,15 @@
   </si>
   <si>
     <t>Phase II HSCT-TMA</t>
+  </si>
+  <si>
+    <t>PEG patent</t>
+  </si>
+  <si>
+    <t>US10035822B2 - 2033 patent, extending to 2035</t>
+  </si>
+  <si>
+    <t>7888323 - expires 2027</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1109,7 @@
   <dimension ref="B2:M18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1386,11 +1395,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E49619-7317-48A8-BEE2-EDC89FDCB0B3}">
   <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AH15" sqref="AH15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2501,59 +2510,59 @@
         <v>118</v>
       </c>
       <c r="N17" s="1">
-        <f>+N16/N18</f>
+        <f t="shared" ref="N17:V17" si="19">+N16/N18</f>
         <v>-1.3296694356814217E-2</v>
       </c>
       <c r="O17" s="1">
-        <f>+O16/O18</f>
+        <f t="shared" si="19"/>
         <v>-1.561209076858227</v>
       </c>
       <c r="P17" s="1">
-        <f>+P16/P18</f>
+        <f t="shared" si="19"/>
         <v>-1.0710516611351371</v>
       </c>
       <c r="Q17" s="1">
-        <f>+Q16/Q18</f>
+        <f t="shared" si="19"/>
         <v>-1.1606424367372727</v>
       </c>
       <c r="R17" s="1">
-        <f>+R16/R18</f>
+        <f t="shared" si="19"/>
         <v>-0.73206744093968601</v>
       </c>
       <c r="S17" s="1">
-        <f>+S16/S18</f>
+        <f t="shared" si="19"/>
         <v>-0.53595159283326699</v>
       </c>
       <c r="T17" s="1">
-        <f>+T16/T18</f>
+        <f t="shared" si="19"/>
         <v>-0.28867510330578494</v>
       </c>
       <c r="U17" s="1">
-        <f>+U16/U18</f>
+        <f t="shared" si="19"/>
         <v>0.31429170971074388</v>
       </c>
       <c r="V17" s="1">
-        <f>+V16/V18</f>
+        <f t="shared" si="19"/>
         <v>0.53500290547520679</v>
       </c>
       <c r="AD17" s="1">
-        <f t="shared" ref="AD17:AH17" si="19">+AD16/AD18</f>
+        <f t="shared" ref="AD17:AH17" si="20">+AD16/AD18</f>
         <v>-4.4495441446603401</v>
       </c>
       <c r="AE17" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.8819271068128493E-2</v>
       </c>
       <c r="AF17" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.3369971435444725</v>
       </c>
       <c r="AG17" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6.2219139764165554</v>
       </c>
       <c r="AH17" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.3183063997299236</v>
       </c>
     </row>
@@ -2607,7 +2616,7 @@
         <v>123.66725</v>
       </c>
       <c r="AH18" s="7">
-        <f t="shared" ref="AH18" si="20">+AG18</f>
+        <f t="shared" ref="AH18" si="21">+AG18</f>
         <v>123.66725</v>
       </c>
     </row>
@@ -2654,31 +2663,31 @@
         <v>0.82587075770414309</v>
       </c>
       <c r="P21" s="23">
-        <f t="shared" ref="P21:V21" si="21">P8/P6</f>
+        <f t="shared" ref="P21:V21" si="22">P8/P6</f>
         <v>0.85</v>
       </c>
       <c r="Q21" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.79704212213698977</v>
       </c>
       <c r="R21" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.86400950676810861</v>
       </c>
       <c r="S21" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.88274441543371041</v>
       </c>
       <c r="T21" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.88429694113168611</v>
       </c>
       <c r="U21" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.9</v>
       </c>
       <c r="V21" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.9</v>
       </c>
       <c r="W21" s="23"/>
@@ -2851,10 +2860,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDEC44E-3A9A-47B3-8A31-8E621049E97B}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2863,12 +2872,12 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -2876,7 +2885,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2884,7 +2893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -2892,7 +2901,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>29</v>
       </c>
@@ -2900,7 +2909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2908,7 +2917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -2916,43 +2925,61 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="10" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" s="10" t="s">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" s="10" t="s">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="10" t="s">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>